<commit_message>
scripts plan and level design .excel & .vsdx
</commit_message>
<xml_diff>
--- a/Doc/地图及关卡设计表格.xlsx
+++ b/Doc/地图及关卡设计表格.xlsx
@@ -4,19 +4,164 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="剧情线索" sheetId="1" r:id="rId1"/>
+    <sheet name="控制机关" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>World1#</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+  <si>
+    <t>剧情线索编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取方式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物品名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物品描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图标注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>破碎的笔记</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这是一则笔记上撕下的一页，字迹已经模糊不堪了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调查房间的书柜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>“这个世界已经到头，必须尽快找到那个地方...”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>房间一角的血迹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>墙上的痕迹已经斑驳，显然已经过了很长时间，但是这是血迹没错</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调查房间的墙壁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>“墙上的痕迹已经斑驳，看来是很久以前留下的，但这是血迹没错...”</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>互动内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制机关编号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图标注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Key 1#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clue 1#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Clue 2#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机关形态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>破解条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机关描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>破解结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>紧锁的门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在World 2#获取钥匙Key 1#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Door 1#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>紧锁的门，找到钥匙才能打开</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打开门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要物品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>钥匙</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>物品地图标注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Door 2#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水底的门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进入World 3#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>World 3#世界水已经干涸，可以直接跳下去开门</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>角色无法进入水底，所以无法开门</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -366,17 +511,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="12.25" customWidth="1"/>
+    <col min="3" max="3" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="60.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
+    <col min="6" max="6" width="66.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -384,4 +601,116 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="7" max="7" width="25.625" customWidth="1"/>
+    <col min="8" max="8" width="44.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>